<commit_message>
some slight modifications to the saving / loading
</commit_message>
<xml_diff>
--- a/fbo_solicitations.xlsx
+++ b/fbo_solicitations.xlsx
@@ -15,41 +15,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>check_office</t>
+  </si>
+  <si>
+    <t>deadline_date</t>
+  </si>
+  <si>
+    <t>check_office_wide</t>
+  </si>
+  <si>
+    <t>announcement_type</t>
+  </si>
+  <si>
+    <t>synopsis</t>
+  </si>
+  <si>
+    <t>program_url</t>
+  </si>
+  <si>
+    <t>opportunity_title</t>
+  </si>
+  <si>
+    <t>check_date</t>
+  </si>
   <si>
     <t>sponsor_number</t>
   </si>
   <si>
-    <t>office</t>
-  </si>
-  <si>
-    <t>check_office</t>
-  </si>
-  <si>
-    <t>deadline_date</t>
-  </si>
-  <si>
-    <t>check_office_wide</t>
-  </si>
-  <si>
-    <t>announcement_type</t>
-  </si>
-  <si>
-    <t>synopsis</t>
-  </si>
-  <si>
-    <t>program_url</t>
-  </si>
-  <si>
-    <t>opportunity_title</t>
-  </si>
-  <si>
-    <t>check_date</t>
-  </si>
-  <si>
-    <t>DARPA-RA-15-32</t>
-  </si>
-  <si>
     <t>DARPA-BAA-14-50</t>
   </si>
   <si>
@@ -68,18 +65,12 @@
     <t>DARPA-BAA-13-37</t>
   </si>
   <si>
-    <t>DARPA-BAA-15-33</t>
-  </si>
-  <si>
     <t>Tactical Technology Office</t>
   </si>
   <si>
     <t>Biological Technologies Office</t>
   </si>
   <si>
-    <t>04/13/2015</t>
-  </si>
-  <si>
     <t>09/04/2015</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>09/17/2013</t>
   </si>
   <si>
-    <t>06/03/2015</t>
-  </si>
-  <si>
     <t>Presolicitation</t>
   </si>
   <si>
@@ -108,17 +96,6 @@
   </si>
   <si>
     <t>Award</t>
-  </si>
-  <si>
-    <t>Added:_x000D_
-Feb 26, 2015 1:37 pm_x000D_
-This solicitation replaces DARPA-RA-15-23._x000D_
-_x000D_
-This Research Announcement (RA) solicits ground-breaking single-investigator proposals from junior faculty for research and development in the areas of Physical Sciences, Engineering, Mathematics, Medicine, Biology, Information and Social Sciences of interest to DARPA's Defense Sciences Office (DSO), Microsystems Technology Office (MTO), and Biological Technology Office (BTO). See the full DARPA-RA-15-32 document attached._x000D_
-_x000D_
-Added:_x000D_
-Apr 09, 2015 11:33 am_x000D_
-Amendment 01: The purpose of this amendment is to make minor revisions to clarify that the Research Announcement (RA) is seeking proposals only from participants/individuals from U.S. institutions of higher education or from U.S. non-profit science and technology research institutions. Proposals are not being sought from foreign organizations.</t>
   </si>
   <si>
     <t>Added:_x000D_
@@ -243,17 +220,6 @@
 		Award Notice for HR0011-15-C-0084 (MIT).</t>
   </si>
   <si>
-    <t>Added:_x000D_
-Apr 15, 2015 12:01 pm_x000D_
-DARPA is soliciting research proposals in the development of navigation-grade inertial measurement units (IMUs) based on microelectromechanical systems (MEMS) technology. The objective of the PRIGM:NGIMU program is to develop navigation-grade inertial measurement units (NGIMU) by integrating MEMS gyroscopes and accelerometers into small form factor IMUs. PRIGM:NGIMU deliverables will provide drop-in replacements for currently deployed tactical-grade MEMS IMUs.  See the DARPA-BAA-15-33 document attached._x000D_
-Added:_x000D_
-May 06, 2015 1:06 pm_x000D_
-The purpose of Amendment No. 01 is to revise the program metrics stipulated at Table 1 (Part II, Section I, Paragraph B) of the Broad Agency Announcement (BAA). All changes made to the BAA are highlighted in yellow - see DARPA-BAA-15-33 Amendment No. 01 document attached to this notice.   All attachments to the BAA remain unchanged.  The proposal deadline remains unchanged.</t>
-  </si>
-  <si>
-    <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=af2d4b77009cc0f207c81632058a4e23&amp;tab=core&amp;_cview=1</t>
-  </si>
-  <si>
     <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=609d9473f9acde0ca577aae2774fb185&amp;tab=core&amp;_cview=1</t>
   </si>
   <si>
@@ -272,12 +238,6 @@
     <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=7610634cc3cbcbb826407a0d208c2515&amp;tab=core&amp;_cview=1</t>
   </si>
   <si>
-    <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=9787bfe46edab65ace878327b1bdbfbd&amp;tab=core&amp;_cview=1</t>
-  </si>
-  <si>
-    <t>Young Faculty Award (YFA)</t>
-  </si>
-  <si>
     <t>Ground X-Vehicle Technologies (GXV-T) Program Technology Development</t>
   </si>
   <si>
@@ -296,9 +256,6 @@
     <t>Living Foundries: 1000 Molecules</t>
   </si>
   <si>
-    <t>Precise Robust Inertial Guidance for Munitions (PRIGM): Navigation-Grade Inertial Measurement Unit (NGIMU)</t>
-  </si>
-  <si>
     <t>DARPA-BAA-14-42</t>
   </si>
   <si>
@@ -311,7 +268,7 @@
     <t>09/09/2016</t>
   </si>
   <si>
-    <t>u'\n\t-\n\t\t'</t>
+    <t>u'-'</t>
   </si>
   <si>
     <t>Added:_x000D_
@@ -720,13 +677,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,258 +714,195 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="b">
+      <c r="J2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" t="b">
+      <c r="J3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="b">
+      <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" t="b">
+      <c r="J4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" t="b">
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
       <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" t="b">
+      <c r="J6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="b">
+      <c r="C7" t="b">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="b">
+      <c r="J7" t="b">
         <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1013,13 +910,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,75 +947,72 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="b">
+      <c r="J3" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added reporting feature (tested)
</commit_message>
<xml_diff>
--- a/fbo_solicitations.xlsx
+++ b/fbo_solicitations.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="notices" sheetId="1" r:id="rId1"/>
-    <sheet name="filtered_notices" sheetId="2" r:id="rId2"/>
+    <sheet name="solicitations" sheetId="1" r:id="rId1"/>
+    <sheet name="filtered_solicitations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="451">
   <si>
     <t>office</t>
   </si>
@@ -1998,6 +1998,9 @@
     <t>DARPA-BAA-14-45</t>
   </si>
   <si>
+    <t>DARPA-BAA-15-04</t>
+  </si>
+  <si>
     <t>Information Innovation Office</t>
   </si>
   <si>
@@ -2751,6 +2754,15 @@
 Under DARPA Broad Agency Announcement No. DARPA-BAA-14-35 Raytheon Company, Missile Sytems, has been awarded a new contract to perform the Multi Azimuth Defense Fast Intercept Round Engagement System (MAD-FIRES) program, Phase 0.</t>
   </si>
   <si>
+    <t>Added:_x000D_
+Jun 30, 2015 11:59 am_x000D_
+Base Award Amount: $585,704_x000D_
+Option (1) Amount: $597,378_x000D_
+Option (2) Amount: $609,286_x000D_
+Option (3) Amount: $621,431_x000D_
+TOTAL Potential Contract Value: $2,413,799</t>
+  </si>
+  <si>
     <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=2a34df9e82288cdd2f04fe502dc9f99a&amp;tab=core&amp;_cview=1</t>
   </si>
   <si>
@@ -2847,6 +2859,9 @@
     <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=e1330b7c4b9bb2450dd9245e53ac7d7a&amp;tab=core&amp;_cview=1</t>
   </si>
   <si>
+    <t>https://www.fbo.gov/index?s=opportunity&amp;mode=form&amp;id=aacab890da9fd621dc0cb5e311b27ee8&amp;tab=core&amp;_cview=1</t>
+  </si>
+  <si>
     <t>Microsystems Technology Office (MTO) Office-Wide Broad Agency Announcement (BAA)</t>
   </si>
   <si>
@@ -2938,6 +2953,9 @@
   </si>
   <si>
     <t>Multi Azimuth Defense Fast Intercept Round Engagement System (MAD-FIRES)</t>
+  </si>
+  <si>
+    <t>Low Resource Languages for Emergent Incidents (LORELEI)</t>
   </si>
 </sst>
 </file>
@@ -5094,7 +5112,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5143,7 +5161,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -5152,13 +5170,13 @@
         <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="I2" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -5172,7 +5190,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -5181,13 +5199,13 @@
         <v>130</v>
       </c>
       <c r="G3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="I3" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -5201,7 +5219,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -5210,10 +5228,10 @@
         <v>131</v>
       </c>
       <c r="G4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I4" t="s">
         <v>262</v>
@@ -5230,7 +5248,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -5239,13 +5257,13 @@
         <v>131</v>
       </c>
       <c r="G5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="I5" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -5259,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -5268,13 +5286,13 @@
         <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="I6" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -5288,22 +5306,22 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="I7" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -5317,7 +5335,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -5326,13 +5344,13 @@
         <v>130</v>
       </c>
       <c r="G8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="I8" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -5346,7 +5364,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -5355,13 +5373,13 @@
         <v>130</v>
       </c>
       <c r="G9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I9" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -5375,7 +5393,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -5384,13 +5402,13 @@
         <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I10" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -5404,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -5413,13 +5431,13 @@
         <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I11" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -5433,7 +5451,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -5442,13 +5460,13 @@
         <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="I12" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -5462,7 +5480,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -5471,13 +5489,13 @@
         <v>131</v>
       </c>
       <c r="G13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I13" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -5491,7 +5509,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -5500,13 +5518,13 @@
         <v>129</v>
       </c>
       <c r="G14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="I14" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -5520,7 +5538,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -5529,13 +5547,13 @@
         <v>131</v>
       </c>
       <c r="G15" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="I15" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -5549,7 +5567,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -5558,13 +5576,13 @@
         <v>130</v>
       </c>
       <c r="G16" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I16" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -5578,7 +5596,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -5587,13 +5605,13 @@
         <v>130</v>
       </c>
       <c r="G17" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="I17" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -5607,7 +5625,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -5616,13 +5634,13 @@
         <v>130</v>
       </c>
       <c r="G18" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I18" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -5636,7 +5654,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -5645,13 +5663,13 @@
         <v>130</v>
       </c>
       <c r="G19" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I19" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -5665,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -5674,13 +5692,13 @@
         <v>130</v>
       </c>
       <c r="G20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="I20" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -5694,22 +5712,22 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G21" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="I21" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -5723,7 +5741,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -5732,13 +5750,13 @@
         <v>131</v>
       </c>
       <c r="G22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="I22" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -5752,7 +5770,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -5761,13 +5779,13 @@
         <v>131</v>
       </c>
       <c r="G23" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I23" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -5781,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -5790,13 +5808,13 @@
         <v>129</v>
       </c>
       <c r="G24" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="I24" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -5810,7 +5828,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -5819,13 +5837,13 @@
         <v>131</v>
       </c>
       <c r="G25" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="I25" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -5839,7 +5857,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -5848,13 +5866,13 @@
         <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="I26" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -5865,13 +5883,13 @@
         <v>330</v>
       </c>
       <c r="B27" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -5880,13 +5898,13 @@
         <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="I27" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -5900,7 +5918,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -5909,13 +5927,13 @@
         <v>131</v>
       </c>
       <c r="G28" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="I28" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -5929,7 +5947,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -5938,13 +5956,13 @@
         <v>130</v>
       </c>
       <c r="G29" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="I29" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -5958,7 +5976,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -5967,13 +5985,13 @@
         <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="I30" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -5990,7 +6008,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -5999,13 +6017,13 @@
         <v>131</v>
       </c>
       <c r="G31" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="I31" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -6022,7 +6040,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -6031,13 +6049,13 @@
         <v>131</v>
       </c>
       <c r="G32" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I32" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -6051,7 +6069,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -6060,15 +6078,44 @@
         <v>131</v>
       </c>
       <c r="G33" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="I33" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="J33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>341</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" t="s">
+        <v>385</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="I34" t="s">
+        <v>450</v>
+      </c>
+      <c r="J34">
         <v>1</v>
       </c>
     </row>
@@ -6106,6 +6153,7 @@
     <hyperlink ref="H31" r:id="rId30"/>
     <hyperlink ref="H32" r:id="rId31"/>
     <hyperlink ref="H33" r:id="rId32"/>
+    <hyperlink ref="H34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>